<commit_message>
Add coin cells, FFC's
</commit_message>
<xml_diff>
--- a/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
+++ b/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="465">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -1376,6 +1376,12 @@
   </si>
   <si>
     <t xml:space="preserve">FFC’s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFC / FPC Jumper Cables WR-FFC 0.5mm Type 2 20P 100mm length. Opposide side contacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR1220 coin cell</t>
   </si>
   <si>
     <t xml:space="preserve">USD-GBP</t>
@@ -1769,7 +1775,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="630" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
+      <selection pane="bottomLeft" activeCell="B85" activeCellId="0" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5503,26 +5509,31 @@
         <v>448</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="s">
+    <row r="84" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="G84" s="0" t="s">
+      <c r="G84" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H84" s="0" t="n">
+      <c r="H84" s="7" t="n">
         <v>687720100002</v>
       </c>
-      <c r="I84" s="0"/>
-      <c r="J84" s="0"/>
-      <c r="K84" s="0"/>
-      <c r="N84" s="0" t="n">
+      <c r="N84" s="7" t="n">
         <f aca="false">$C$94*D84</f>
         <v>0</v>
       </c>
-      <c r="R84" s="0"/>
+      <c r="U84" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="V84" s="7" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="0" t="s">
+        <v>453</v>
+      </c>
       <c r="N85" s="0" t="n">
         <f aca="false">$C$94*D85</f>
         <v>0</v>
@@ -5554,7 +5565,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>1.38</v>
@@ -5562,7 +5573,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>8</v>
@@ -5570,7 +5581,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>70</v>
@@ -5578,7 +5589,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>85</v>
@@ -5586,30 +5597,30 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="10" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="7" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="14" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="23" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5624,7 +5635,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="25" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BOM to include more mechanical parts
</commit_message>
<xml_diff>
--- a/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
+++ b/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="466">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -1373,6 +1373,9 @@
   </si>
   <si>
     <t xml:space="preserve">TR00009928-000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screw M2x4mm</t>
   </si>
   <si>
     <t xml:space="preserve">FFC’s</t>
@@ -1770,12 +1773,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ104"/>
+  <dimension ref="A1:AMJ105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="630" topLeftCell="A13" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B85" activeCellId="0" sqref="B85"/>
+      <selection pane="bottomLeft" activeCell="B84" activeCellId="0" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1909,7 +1912,7 @@
         <v>30</v>
       </c>
       <c r="N2" s="8" t="n">
-        <f aca="false">$C$94*D2</f>
+        <f aca="false">$C$95*D2</f>
         <v>85</v>
       </c>
       <c r="O2" s="8" t="n">
@@ -1958,7 +1961,7 @@
         <v>39</v>
       </c>
       <c r="N3" s="8" t="n">
-        <f aca="false">$C$94*D3</f>
+        <f aca="false">$C$95*D3</f>
         <v>425</v>
       </c>
       <c r="O3" s="8" t="n">
@@ -2006,7 +2009,7 @@
         <v>45</v>
       </c>
       <c r="N4" s="8" t="n">
-        <f aca="false">$C$94*D4</f>
+        <f aca="false">$C$95*D4</f>
         <v>255</v>
       </c>
       <c r="O4" s="8" t="n">
@@ -2054,7 +2057,7 @@
         <v>52</v>
       </c>
       <c r="N5" s="11" t="n">
-        <f aca="false">$C$94*D5</f>
+        <f aca="false">$C$95*D5</f>
         <v>255</v>
       </c>
       <c r="O5" s="11" t="n">
@@ -2099,7 +2102,7 @@
         <v>57</v>
       </c>
       <c r="N6" s="11" t="n">
-        <f aca="false">$C$94*D6</f>
+        <f aca="false">$C$95*D6</f>
         <v>85</v>
       </c>
       <c r="O6" s="11" t="n">
@@ -2144,7 +2147,7 @@
         <v>62</v>
       </c>
       <c r="N7" s="11" t="n">
-        <f aca="false">$C$94*D7</f>
+        <f aca="false">$C$95*D7</f>
         <v>170</v>
       </c>
       <c r="O7" s="11" t="n">
@@ -2192,7 +2195,7 @@
         <v>1907351</v>
       </c>
       <c r="N8" s="8" t="n">
-        <f aca="false">$C$94*D8</f>
+        <f aca="false">$C$95*D8</f>
         <v>340</v>
       </c>
       <c r="O8" s="8" t="n">
@@ -2260,7 +2263,7 @@
         <v>74</v>
       </c>
       <c r="N10" s="11" t="n">
-        <f aca="false">$C$94*D10</f>
+        <f aca="false">$C$95*D10</f>
         <v>255</v>
       </c>
       <c r="O10" s="11" t="n">
@@ -2328,7 +2331,7 @@
         <v>81</v>
       </c>
       <c r="N12" s="11" t="n">
-        <f aca="false">$C$94*D12</f>
+        <f aca="false">$C$95*D12</f>
         <v>85</v>
       </c>
       <c r="O12" s="11" t="n">
@@ -2373,7 +2376,7 @@
         <v>85</v>
       </c>
       <c r="N13" s="11" t="n">
-        <f aca="false">$C$94*D13</f>
+        <f aca="false">$C$95*D13</f>
         <v>1190</v>
       </c>
       <c r="O13" s="11" t="n">
@@ -2421,7 +2424,7 @@
         <v>91</v>
       </c>
       <c r="N14" s="11" t="n">
-        <f aca="false">$C$94*D14</f>
+        <f aca="false">$C$95*D14</f>
         <v>425</v>
       </c>
       <c r="O14" s="11" t="n">
@@ -2466,7 +2469,7 @@
         <v>95</v>
       </c>
       <c r="N15" s="11" t="n">
-        <f aca="false">$C$94*D15</f>
+        <f aca="false">$C$95*D15</f>
         <v>425</v>
       </c>
       <c r="O15" s="11" t="n">
@@ -2511,7 +2514,7 @@
         <v>99</v>
       </c>
       <c r="N16" s="11" t="n">
-        <f aca="false">$C$94*D16</f>
+        <f aca="false">$C$95*D16</f>
         <v>510</v>
       </c>
       <c r="O16" s="11" t="n">
@@ -2559,7 +2562,7 @@
         <v>107</v>
       </c>
       <c r="N17" s="8" t="n">
-        <f aca="false">$C$94*D17</f>
+        <f aca="false">$C$95*D17</f>
         <v>85</v>
       </c>
       <c r="O17" s="8" t="n">
@@ -2613,7 +2616,7 @@
         <v>107</v>
       </c>
       <c r="N18" s="8" t="n">
-        <f aca="false">$C$94*D18</f>
+        <f aca="false">$C$95*D18</f>
         <v>85</v>
       </c>
       <c r="O18" s="8" t="n">
@@ -2670,7 +2673,7 @@
         <v>107</v>
       </c>
       <c r="N19" s="8" t="n">
-        <f aca="false">$C$94*D19</f>
+        <f aca="false">$C$95*D19</f>
         <v>85</v>
       </c>
       <c r="O19" s="8" t="n">
@@ -2727,7 +2730,7 @@
         <v>107</v>
       </c>
       <c r="N20" s="8" t="n">
-        <f aca="false">$C$94*D20</f>
+        <f aca="false">$C$95*D20</f>
         <v>85</v>
       </c>
       <c r="O20" s="8" t="n">
@@ -2781,7 +2784,7 @@
         <v>107</v>
       </c>
       <c r="N21" s="8" t="n">
-        <f aca="false">$C$94*D21</f>
+        <f aca="false">$C$95*D21</f>
         <v>85</v>
       </c>
       <c r="O21" s="8" t="n">
@@ -2835,7 +2838,7 @@
         <v>107</v>
       </c>
       <c r="N22" s="8" t="n">
-        <f aca="false">$C$94*D22</f>
+        <f aca="false">$C$95*D22</f>
         <v>85</v>
       </c>
       <c r="O22" s="8" t="n">
@@ -2889,7 +2892,7 @@
         <v>107</v>
       </c>
       <c r="N23" s="8" t="n">
-        <f aca="false">$C$94*D23</f>
+        <f aca="false">$C$95*D23</f>
         <v>170</v>
       </c>
       <c r="O23" s="8" t="n">
@@ -2946,7 +2949,7 @@
         <v>107</v>
       </c>
       <c r="N24" s="8" t="n">
-        <f aca="false">$C$94*D24</f>
+        <f aca="false">$C$95*D24</f>
         <v>170</v>
       </c>
       <c r="O24" s="8" t="n">
@@ -2997,7 +3000,7 @@
         <v>155</v>
       </c>
       <c r="N25" s="7" t="n">
-        <f aca="false">$C$94*D25</f>
+        <f aca="false">$C$95*D25</f>
         <v>85</v>
       </c>
       <c r="O25" s="8" t="n">
@@ -3042,7 +3045,7 @@
         <v>162</v>
       </c>
       <c r="N26" s="8" t="n">
-        <f aca="false">$C$94*D26</f>
+        <f aca="false">$C$95*D26</f>
         <v>85</v>
       </c>
       <c r="O26" s="8" t="n">
@@ -3150,7 +3153,7 @@
         <v>107</v>
       </c>
       <c r="N28" s="8" t="n">
-        <f aca="false">$C$94*D28</f>
+        <f aca="false">$C$95*D28</f>
         <v>85</v>
       </c>
       <c r="O28" s="8" t="n">
@@ -3207,7 +3210,7 @@
         <v>107</v>
       </c>
       <c r="N29" s="15" t="n">
-        <f aca="false">$C$94*D29</f>
+        <f aca="false">$C$95*D29</f>
         <v>85</v>
       </c>
       <c r="O29" s="15" t="n">
@@ -3271,7 +3274,7 @@
         <v>107</v>
       </c>
       <c r="N30" s="15" t="n">
-        <f aca="false">$C$94*D30</f>
+        <f aca="false">$C$95*D30</f>
         <v>85</v>
       </c>
       <c r="O30" s="15" t="n">
@@ -3331,7 +3334,7 @@
         <v>107</v>
       </c>
       <c r="N31" s="8" t="n">
-        <f aca="false">$C$94*D31</f>
+        <f aca="false">$C$95*D31</f>
         <v>85</v>
       </c>
       <c r="O31" s="8" t="n">
@@ -3388,7 +3391,7 @@
         <v>107</v>
       </c>
       <c r="N32" s="15" t="n">
-        <f aca="false">$C$94*D32</f>
+        <f aca="false">$C$95*D32</f>
         <v>170</v>
       </c>
       <c r="O32" s="15" t="n">
@@ -3445,7 +3448,7 @@
         <v>214</v>
       </c>
       <c r="N33" s="15" t="n">
-        <f aca="false">$C$94*D33</f>
+        <f aca="false">$C$95*D33</f>
         <v>85</v>
       </c>
       <c r="O33" s="15" t="n">
@@ -3505,7 +3508,7 @@
         <v>31</v>
       </c>
       <c r="N34" s="8" t="n">
-        <f aca="false">$C$94*D34</f>
+        <f aca="false">$C$95*D34</f>
         <v>85</v>
       </c>
       <c r="O34" s="8" t="n">
@@ -3565,7 +3568,7 @@
         <v>31</v>
       </c>
       <c r="N35" s="8" t="n">
-        <f aca="false">$C$94*D35</f>
+        <f aca="false">$C$95*D35</f>
         <v>85</v>
       </c>
       <c r="O35" s="8" t="n">
@@ -3625,7 +3628,7 @@
         <v>107</v>
       </c>
       <c r="N36" s="8" t="n">
-        <f aca="false">$C$94*D36</f>
+        <f aca="false">$C$95*D36</f>
         <v>255</v>
       </c>
       <c r="O36" s="8" t="n">
@@ -3776,7 +3779,7 @@
         <v>107</v>
       </c>
       <c r="N39" s="8" t="n">
-        <f aca="false">$C$94*D39</f>
+        <f aca="false">$C$95*D39</f>
         <v>170</v>
       </c>
       <c r="O39" s="8" t="n">
@@ -3830,7 +3833,7 @@
         <v>107</v>
       </c>
       <c r="N40" s="8" t="n">
-        <f aca="false">$C$94*D40</f>
+        <f aca="false">$C$95*D40</f>
         <v>255</v>
       </c>
       <c r="O40" s="8" t="n">
@@ -3884,7 +3887,7 @@
         <v>107</v>
       </c>
       <c r="N41" s="8" t="n">
-        <f aca="false">$C$94*D41</f>
+        <f aca="false">$C$95*D41</f>
         <v>680</v>
       </c>
       <c r="O41" s="8" t="n">
@@ -3935,7 +3938,7 @@
         <v>273</v>
       </c>
       <c r="N42" s="11" t="n">
-        <f aca="false">$C$94*D42</f>
+        <f aca="false">$C$95*D42</f>
         <v>170</v>
       </c>
       <c r="P42" s="11" t="n">
@@ -4003,7 +4006,7 @@
         <v>279</v>
       </c>
       <c r="N44" s="11" t="n">
-        <f aca="false">$C$94*D44</f>
+        <f aca="false">$C$95*D44</f>
         <v>170</v>
       </c>
       <c r="O44" s="11" t="n">
@@ -4048,7 +4051,7 @@
         <v>285</v>
       </c>
       <c r="N45" s="11" t="n">
-        <f aca="false">$C$94*D45</f>
+        <f aca="false">$C$95*D45</f>
         <v>170</v>
       </c>
       <c r="O45" s="11" t="n">
@@ -4093,7 +4096,7 @@
         <v>290</v>
       </c>
       <c r="N46" s="11" t="n">
-        <f aca="false">$C$94*D46</f>
+        <f aca="false">$C$95*D46</f>
         <v>765</v>
       </c>
       <c r="O46" s="11" t="n">
@@ -4141,7 +4144,7 @@
         <v>295</v>
       </c>
       <c r="N47" s="11" t="n">
-        <f aca="false">$C$94*D47</f>
+        <f aca="false">$C$95*D47</f>
         <v>85</v>
       </c>
       <c r="O47" s="11" t="n">
@@ -4215,7 +4218,7 @@
         <v>300</v>
       </c>
       <c r="N49" s="11" t="n">
-        <f aca="false">$C$94*D49</f>
+        <f aca="false">$C$95*D49</f>
         <v>765</v>
       </c>
       <c r="O49" s="11" t="n">
@@ -4248,7 +4251,7 @@
         <v>303</v>
       </c>
       <c r="N50" s="13" t="n">
-        <f aca="false">$C$94*D50</f>
+        <f aca="false">$C$95*D50</f>
         <v>0</v>
       </c>
       <c r="U50" s="13" t="s">
@@ -4275,7 +4278,7 @@
         <v>305</v>
       </c>
       <c r="N51" s="13" t="n">
-        <f aca="false">$C$94*D51</f>
+        <f aca="false">$C$95*D51</f>
         <v>0</v>
       </c>
       <c r="U51" s="13" t="s">
@@ -4314,7 +4317,7 @@
         <v>309</v>
       </c>
       <c r="N52" s="11" t="n">
-        <f aca="false">$C$94*D52</f>
+        <f aca="false">$C$95*D52</f>
         <v>85</v>
       </c>
       <c r="O52" s="11" t="n">
@@ -4359,7 +4362,7 @@
         <v>314</v>
       </c>
       <c r="N53" s="11" t="n">
-        <f aca="false">$C$94*D53</f>
+        <f aca="false">$C$95*D53</f>
         <v>340</v>
       </c>
       <c r="O53" s="11" t="n">
@@ -4404,7 +4407,7 @@
         <v>319</v>
       </c>
       <c r="N54" s="11" t="n">
-        <f aca="false">$C$94*D54</f>
+        <f aca="false">$C$95*D54</f>
         <v>170</v>
       </c>
       <c r="O54" s="11" t="n">
@@ -4449,7 +4452,7 @@
         <v>325</v>
       </c>
       <c r="N55" s="11" t="n">
-        <f aca="false">$C$94*D55</f>
+        <f aca="false">$C$95*D55</f>
         <v>170</v>
       </c>
       <c r="O55" s="11" t="n">
@@ -4494,7 +4497,7 @@
         <v>330</v>
       </c>
       <c r="N56" s="11" t="n">
-        <f aca="false">$C$94*D56</f>
+        <f aca="false">$C$95*D56</f>
         <v>595</v>
       </c>
       <c r="O56" s="11" t="n">
@@ -4536,7 +4539,7 @@
         <v>334</v>
       </c>
       <c r="N57" s="10" t="n">
-        <f aca="false">$C$94*D57</f>
+        <f aca="false">$C$95*D57</f>
         <v>1020</v>
       </c>
       <c r="O57" s="10" t="n">
@@ -4579,7 +4582,7 @@
         <v>342</v>
       </c>
       <c r="N58" s="15" t="n">
-        <f aca="false">$C$94*D58</f>
+        <f aca="false">$C$95*D58</f>
         <v>170</v>
       </c>
       <c r="O58" s="15" t="n">
@@ -4634,7 +4637,7 @@
         <v>107</v>
       </c>
       <c r="N59" s="15" t="n">
-        <f aca="false">$C$94*D59</f>
+        <f aca="false">$C$95*D59</f>
         <v>340</v>
       </c>
       <c r="O59" s="15" t="n">
@@ -4692,7 +4695,7 @@
         <v>107</v>
       </c>
       <c r="N60" s="8" t="n">
-        <f aca="false">$C$94*D60</f>
+        <f aca="false">$C$95*D60</f>
         <v>170</v>
       </c>
       <c r="O60" s="8" t="n">
@@ -4749,7 +4752,7 @@
         <v>162</v>
       </c>
       <c r="N61" s="8" t="n">
-        <f aca="false">$C$94*D61</f>
+        <f aca="false">$C$95*D61</f>
         <v>85</v>
       </c>
       <c r="O61" s="8" t="n">
@@ -4809,7 +4812,7 @@
         <v>162</v>
       </c>
       <c r="N62" s="11" t="n">
-        <f aca="false">$C$94*D62</f>
+        <f aca="false">$C$95*D62</f>
         <v>85</v>
       </c>
       <c r="O62" s="11" t="n">
@@ -4860,7 +4863,7 @@
         <v>162</v>
       </c>
       <c r="N63" s="15" t="n">
-        <f aca="false">$C$94*D63</f>
+        <f aca="false">$C$95*D63</f>
         <v>85</v>
       </c>
       <c r="O63" s="15" t="n">
@@ -4920,7 +4923,7 @@
         <v>162</v>
       </c>
       <c r="N64" s="11" t="n">
-        <f aca="false">$C$94*D64</f>
+        <f aca="false">$C$95*D64</f>
         <v>85</v>
       </c>
       <c r="O64" s="11" t="n">
@@ -5007,7 +5010,7 @@
         <v>107</v>
       </c>
       <c r="N66" s="8" t="n">
-        <f aca="false">$C$94*D66</f>
+        <f aca="false">$C$95*D66</f>
         <v>425</v>
       </c>
       <c r="O66" s="8" t="n">
@@ -5064,7 +5067,7 @@
         <v>172</v>
       </c>
       <c r="N67" s="15" t="n">
-        <f aca="false">$C$94*D67</f>
+        <f aca="false">$C$95*D67</f>
         <v>170</v>
       </c>
       <c r="O67" s="15" t="n">
@@ -5121,7 +5124,7 @@
         <v>172</v>
       </c>
       <c r="N68" s="15" t="n">
-        <f aca="false">$C$94*D68</f>
+        <f aca="false">$C$95*D68</f>
         <v>170</v>
       </c>
       <c r="O68" s="15" t="n">
@@ -5193,7 +5196,7 @@
       <c r="J70" s="0"/>
       <c r="K70" s="0"/>
       <c r="N70" s="0" t="n">
-        <f aca="false">$C$94*D70</f>
+        <f aca="false">$C$95*D70</f>
         <v>0</v>
       </c>
       <c r="R70" s="0"/>
@@ -5204,7 +5207,7 @@
       <c r="J71" s="0"/>
       <c r="K71" s="0"/>
       <c r="N71" s="0" t="n">
-        <f aca="false">$C$94*D71</f>
+        <f aca="false">$C$95*D71</f>
         <v>0</v>
       </c>
       <c r="R71" s="0"/>
@@ -5230,7 +5233,7 @@
         <v>2300599</v>
       </c>
       <c r="N72" s="23" t="n">
-        <f aca="false">$C$94*D72</f>
+        <f aca="false">$C$95*D72</f>
         <v>255</v>
       </c>
       <c r="O72" s="23" t="n">
@@ -5259,7 +5262,7 @@
         <v>423</v>
       </c>
       <c r="N73" s="0" t="n">
-        <f aca="false">$C$94*D73</f>
+        <f aca="false">$C$95*D73</f>
         <v>0</v>
       </c>
     </row>
@@ -5271,7 +5274,7 @@
         <v>422</v>
       </c>
       <c r="N74" s="0" t="n">
-        <f aca="false">$C$94*D74</f>
+        <f aca="false">$C$95*D74</f>
         <v>0</v>
       </c>
     </row>
@@ -5294,7 +5297,7 @@
       <c r="J75" s="22"/>
       <c r="K75" s="22"/>
       <c r="N75" s="7" t="n">
-        <f aca="false">$C$94*D75</f>
+        <f aca="false">$C$95*D75</f>
         <v>425</v>
       </c>
       <c r="O75" s="7" t="n">
@@ -5448,7 +5451,7 @@
         <v>443</v>
       </c>
       <c r="N81" s="0" t="n">
-        <f aca="false">$C$94*D81</f>
+        <f aca="false">$C$95*D81</f>
         <v>85</v>
       </c>
       <c r="P81" s="0" t="n">
@@ -5475,7 +5478,7 @@
         <v>447</v>
       </c>
       <c r="N82" s="0" t="n">
-        <f aca="false">$C$94*D82</f>
+        <f aca="false">$C$95*D82</f>
         <v>510</v>
       </c>
       <c r="O82" s="0" t="n">
@@ -5502,81 +5505,78 @@
         <v>450</v>
       </c>
       <c r="N83" s="0" t="n">
-        <f aca="false">$C$94*D83</f>
+        <f aca="false">$C$95*D83</f>
         <v>510</v>
       </c>
       <c r="U83" s="0" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="84" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="7" t="s">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="0" t="s">
         <v>451</v>
       </c>
-      <c r="G84" s="7" t="s">
+    </row>
+    <row r="85" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="G85" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H84" s="7" t="n">
+      <c r="H85" s="7" t="n">
         <v>687720100002</v>
       </c>
-      <c r="N84" s="7" t="n">
-        <f aca="false">$C$94*D84</f>
+      <c r="N85" s="7" t="n">
+        <f aca="false">$C$95*D85</f>
         <v>0</v>
       </c>
-      <c r="U84" s="7" t="s">
+      <c r="U85" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="V84" s="7" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0" t="s">
+      <c r="V85" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="N85" s="0" t="n">
-        <f aca="false">$C$94*D85</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="0" t="s">
+        <v>454</v>
+      </c>
       <c r="N86" s="0" t="n">
-        <f aca="false">$C$94*D86</f>
+        <f aca="false">$C$95*D86</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N87" s="0" t="n">
-        <f aca="false">$C$94*D87</f>
+        <f aca="false">$C$95*D87</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N88" s="0" t="n">
-        <f aca="false">$C$94*D88</f>
+        <f aca="false">$C$95*D88</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N89" s="0" t="n">
-        <f aca="false">$C$94*D89</f>
+        <f aca="false">$C$95*D89</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="D90" s="0" t="n">
+      <c r="N90" s="0" t="n">
+        <f aca="false">$C$95*D90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="D91" s="0" t="n">
         <v>1.38</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="C92" s="0" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5584,7 +5584,7 @@
         <v>456</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5592,54 +5592,62 @@
         <v>457</v>
       </c>
       <c r="C94" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C95" s="0" t="n">
         <v>85</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="C96" s="0" t="s">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="0" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="10" t="s">
+      <c r="C97" s="0" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="7" t="s">
+      <c r="B99" s="10" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="7" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="23" t="s">
+      <c r="B101" s="14" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="18" t="s">
+      <c r="B102" s="23" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="18" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="12" t="s">
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="25" t="s">
-        <v>464</v>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="25" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P85:P89 P2:P78 P80:P83">
+  <conditionalFormatting sqref="P86:P90 P2:P78 P80:P84">
     <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>'safeproject-panel-r2-bom-21340'!N2</formula>
     </cfRule>

</xml_diff>

<commit_message>
BOM update - check in some more parts
</commit_message>
<xml_diff>
--- a/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
+++ b/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
@@ -1791,9 +1791,9 @@
   <dimension ref="A1:AMJ106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="A36" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="630" topLeftCell="A5" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+      <selection pane="bottomLeft" activeCell="P78" activeCellId="0" sqref="P78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4092,6 +4092,9 @@
       <c r="O49" s="20" t="n">
         <v>5000</v>
       </c>
+      <c r="P49" s="20" t="n">
+        <v>5000</v>
+      </c>
       <c r="U49" s="20" t="s">
         <v>40</v>
       </c>
@@ -4128,6 +4131,9 @@
         <v>255</v>
       </c>
       <c r="O50" s="20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="P50" s="20" t="n">
         <v>5000</v>
       </c>
       <c r="AMI50" s="21"/>
@@ -5384,6 +5390,12 @@
       <c r="N84" s="0" t="n">
         <f aca="false">$B$96*C84</f>
         <v>510</v>
+      </c>
+      <c r="O84" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P84" s="0" t="n">
+        <v>1000</v>
       </c>
       <c r="U84" s="0" t="s">
         <v>453</v>

</xml_diff>

<commit_message>
Add a few more details to BoM
</commit_message>
<xml_diff>
--- a/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
+++ b/r3/build/bugg-panel-r3-bom/bugg-panel-r3-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="476">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -940,12 +940,6 @@
     <t xml:space="preserve">197-8062</t>
   </si>
   <si>
-    <t xml:space="preserve">R21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNP 29.4k</t>
-  </si>
-  <si>
     <t xml:space="preserve">R22</t>
   </si>
   <si>
@@ -1285,6 +1279,9 @@
     <t xml:space="preserve">Reeled</t>
   </si>
   <si>
+    <t xml:space="preserve">//</t>
+  </si>
+  <si>
     <t xml:space="preserve">In hand</t>
   </si>
   <si>
@@ -1303,12 +1300,15 @@
     <t xml:space="preserve">Automotion</t>
   </si>
   <si>
-    <t xml:space="preserve">10mm</t>
+    <t xml:space="preserve">P0161.030-010-B2</t>
   </si>
   <si>
     <t xml:space="preserve">Locking washers</t>
   </si>
   <si>
+    <t xml:space="preserve">P0168.030-A2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Molex Clik-Mate crimp contact</t>
   </si>
   <si>
@@ -1402,6 +1402,18 @@
     <t xml:space="preserve">CR1220 coin cell</t>
   </si>
   <si>
+    <t xml:space="preserve">Antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taoglas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FXUB63.07.0150C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">960-FXUB63.07.0150C </t>
+  </si>
+  <si>
     <t xml:space="preserve">USD-GBP</t>
   </si>
   <si>
@@ -1433,6 +1445,9 @@
   </si>
   <si>
     <t xml:space="preserve">Order from RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order from Manufacturer (See Manufacturer column)</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1603,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1693,6 +1708,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1790,22 +1809,22 @@
   </sheetPr>
   <dimension ref="A1:AMJ106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="A5" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P78" activeCellId="0" sqref="P78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="630" topLeftCell="A68" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="A103" activeCellId="0" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.35"/>
@@ -1924,7 +1943,7 @@
         <v>30</v>
       </c>
       <c r="N2" s="7" t="n">
-        <f aca="false">$B$96*C2</f>
+        <f aca="false">$B$95*C2</f>
         <v>85</v>
       </c>
       <c r="O2" s="7" t="n">
@@ -1970,14 +1989,14 @@
         <v>39</v>
       </c>
       <c r="N3" s="7" t="n">
-        <f aca="false">$B$96*C3</f>
+        <f aca="false">$B$95*C3</f>
         <v>425</v>
       </c>
       <c r="O3" s="7" t="n">
         <v>500</v>
       </c>
       <c r="P3" s="7" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>40</v>
@@ -2014,14 +2033,14 @@
         <v>45</v>
       </c>
       <c r="N4" s="7" t="n">
-        <f aca="false">$B$96*C4</f>
+        <f aca="false">$B$95*C4</f>
         <v>255</v>
       </c>
       <c r="O4" s="7" t="n">
         <v>500</v>
       </c>
       <c r="P4" s="7" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>40</v>
@@ -2058,7 +2077,7 @@
         <v>52</v>
       </c>
       <c r="N5" s="10" t="n">
-        <f aca="false">$B$96*C5</f>
+        <f aca="false">$B$95*C5</f>
         <v>255</v>
       </c>
       <c r="O5" s="10" t="n">
@@ -2100,7 +2119,7 @@
         <v>57</v>
       </c>
       <c r="N6" s="10" t="n">
-        <f aca="false">$B$96*C6</f>
+        <f aca="false">$B$95*C6</f>
         <v>85</v>
       </c>
       <c r="O6" s="10" t="n">
@@ -2142,7 +2161,7 @@
         <v>62</v>
       </c>
       <c r="N7" s="10" t="n">
-        <f aca="false">$B$96*C7</f>
+        <f aca="false">$B$95*C7</f>
         <v>170</v>
       </c>
       <c r="O7" s="10" t="n">
@@ -2187,11 +2206,14 @@
         <v>1907351</v>
       </c>
       <c r="N8" s="7" t="n">
-        <f aca="false">$B$96*C8</f>
+        <f aca="false">$B$95*C8</f>
         <v>340</v>
       </c>
       <c r="O8" s="7" t="n">
         <v>400</v>
+      </c>
+      <c r="P8" s="7" t="n">
+        <v>500</v>
       </c>
       <c r="AMI8" s="9"/>
       <c r="AMJ8" s="0"/>
@@ -2248,7 +2270,7 @@
         <v>74</v>
       </c>
       <c r="N10" s="10" t="n">
-        <f aca="false">$B$96*C10</f>
+        <f aca="false">$B$95*C10</f>
         <v>255</v>
       </c>
       <c r="O10" s="10" t="n">
@@ -2310,7 +2332,7 @@
         <v>81</v>
       </c>
       <c r="N12" s="10" t="n">
-        <f aca="false">$B$96*C12</f>
+        <f aca="false">$B$95*C12</f>
         <v>85</v>
       </c>
       <c r="O12" s="10" t="n">
@@ -2352,7 +2374,7 @@
         <v>85</v>
       </c>
       <c r="N13" s="10" t="n">
-        <f aca="false">$B$96*C13</f>
+        <f aca="false">$B$95*C13</f>
         <v>1190</v>
       </c>
       <c r="O13" s="10" t="n">
@@ -2397,7 +2419,7 @@
         <v>91</v>
       </c>
       <c r="N14" s="10" t="n">
-        <f aca="false">$B$96*C14</f>
+        <f aca="false">$B$95*C14</f>
         <v>425</v>
       </c>
       <c r="O14" s="10" t="n">
@@ -2439,7 +2461,7 @@
         <v>95</v>
       </c>
       <c r="N15" s="10" t="n">
-        <f aca="false">$B$96*C15</f>
+        <f aca="false">$B$95*C15</f>
         <v>425</v>
       </c>
       <c r="O15" s="10" t="n">
@@ -2481,7 +2503,7 @@
         <v>99</v>
       </c>
       <c r="N16" s="10" t="n">
-        <f aca="false">$B$96*C16</f>
+        <f aca="false">$B$95*C16</f>
         <v>510</v>
       </c>
       <c r="O16" s="10" t="n">
@@ -2526,7 +2548,7 @@
         <v>107</v>
       </c>
       <c r="N17" s="7" t="n">
-        <f aca="false">$B$96*C17</f>
+        <f aca="false">$B$95*C17</f>
         <v>85</v>
       </c>
       <c r="O17" s="7" t="n">
@@ -2577,7 +2599,7 @@
         <v>107</v>
       </c>
       <c r="N18" s="7" t="n">
-        <f aca="false">$B$96*C18</f>
+        <f aca="false">$B$95*C18</f>
         <v>85</v>
       </c>
       <c r="O18" s="7" t="n">
@@ -2631,7 +2653,7 @@
         <v>107</v>
       </c>
       <c r="N19" s="7" t="n">
-        <f aca="false">$B$96*C19</f>
+        <f aca="false">$B$95*C19</f>
         <v>85</v>
       </c>
       <c r="O19" s="7" t="n">
@@ -2685,7 +2707,7 @@
         <v>107</v>
       </c>
       <c r="N20" s="7" t="n">
-        <f aca="false">$B$96*C20</f>
+        <f aca="false">$B$95*C20</f>
         <v>85</v>
       </c>
       <c r="O20" s="7" t="n">
@@ -2736,7 +2758,7 @@
         <v>107</v>
       </c>
       <c r="N21" s="7" t="n">
-        <f aca="false">$B$96*C21</f>
+        <f aca="false">$B$95*C21</f>
         <v>85</v>
       </c>
       <c r="O21" s="7" t="n">
@@ -2787,7 +2809,7 @@
         <v>107</v>
       </c>
       <c r="N22" s="7" t="n">
-        <f aca="false">$B$96*C22</f>
+        <f aca="false">$B$95*C22</f>
         <v>85</v>
       </c>
       <c r="O22" s="7" t="n">
@@ -2838,7 +2860,7 @@
         <v>107</v>
       </c>
       <c r="N23" s="7" t="n">
-        <f aca="false">$B$96*C23</f>
+        <f aca="false">$B$95*C23</f>
         <v>170</v>
       </c>
       <c r="O23" s="7" t="n">
@@ -2892,7 +2914,7 @@
         <v>107</v>
       </c>
       <c r="N24" s="7" t="n">
-        <f aca="false">$B$96*C24</f>
+        <f aca="false">$B$95*C24</f>
         <v>170</v>
       </c>
       <c r="O24" s="7" t="n">
@@ -2940,10 +2962,13 @@
         <v>155</v>
       </c>
       <c r="N25" s="7" t="n">
-        <f aca="false">$B$96*C25</f>
+        <f aca="false">$B$95*C25</f>
         <v>85</v>
       </c>
       <c r="O25" s="7" t="n">
+        <v>85</v>
+      </c>
+      <c r="P25" s="7" t="n">
         <v>85</v>
       </c>
       <c r="U25" s="7" t="s">
@@ -2981,7 +3006,7 @@
         <v>162</v>
       </c>
       <c r="N26" s="7" t="n">
-        <f aca="false">$B$96*C26</f>
+        <f aca="false">$B$95*C26</f>
         <v>85</v>
       </c>
       <c r="O26" s="7" t="n">
@@ -3088,7 +3113,7 @@
         <v>107</v>
       </c>
       <c r="N28" s="7" t="n">
-        <f aca="false">$B$96*C28</f>
+        <f aca="false">$B$95*C28</f>
         <v>85</v>
       </c>
       <c r="O28" s="7" t="n">
@@ -3142,7 +3167,7 @@
         <v>107</v>
       </c>
       <c r="N29" s="13" t="n">
-        <f aca="false">$B$96*C29</f>
+        <f aca="false">$B$95*C29</f>
         <v>85</v>
       </c>
       <c r="O29" s="13" t="n">
@@ -3203,7 +3228,7 @@
         <v>107</v>
       </c>
       <c r="N30" s="13" t="n">
-        <f aca="false">$B$96*C30</f>
+        <f aca="false">$B$95*C30</f>
         <v>85</v>
       </c>
       <c r="O30" s="13" t="n">
@@ -3260,7 +3285,7 @@
         <v>107</v>
       </c>
       <c r="N31" s="7" t="n">
-        <f aca="false">$B$96*C31</f>
+        <f aca="false">$B$95*C31</f>
         <v>85</v>
       </c>
       <c r="O31" s="7" t="n">
@@ -3314,7 +3339,7 @@
         <v>107</v>
       </c>
       <c r="N32" s="13" t="n">
-        <f aca="false">$B$96*C32</f>
+        <f aca="false">$B$95*C32</f>
         <v>170</v>
       </c>
       <c r="O32" s="13" t="n">
@@ -3368,7 +3393,7 @@
         <v>214</v>
       </c>
       <c r="N33" s="13" t="n">
-        <f aca="false">$B$96*C33</f>
+        <f aca="false">$B$95*C33</f>
         <v>85</v>
       </c>
       <c r="O33" s="13" t="n">
@@ -3425,7 +3450,7 @@
         <v>31</v>
       </c>
       <c r="N34" s="7" t="n">
-        <f aca="false">$B$96*C34</f>
+        <f aca="false">$B$95*C34</f>
         <v>85</v>
       </c>
       <c r="O34" s="7" t="n">
@@ -3482,7 +3507,7 @@
         <v>31</v>
       </c>
       <c r="N35" s="7" t="n">
-        <f aca="false">$B$96*C35</f>
+        <f aca="false">$B$95*C35</f>
         <v>85</v>
       </c>
       <c r="O35" s="7" t="n">
@@ -3539,7 +3564,7 @@
         <v>107</v>
       </c>
       <c r="N36" s="7" t="n">
-        <f aca="false">$B$96*C36</f>
+        <f aca="false">$B$95*C36</f>
         <v>255</v>
       </c>
       <c r="O36" s="7" t="n">
@@ -3683,7 +3708,7 @@
         <v>107</v>
       </c>
       <c r="N39" s="7" t="n">
-        <f aca="false">$B$96*C39</f>
+        <f aca="false">$B$95*C39</f>
         <v>170</v>
       </c>
       <c r="O39" s="7" t="n">
@@ -3734,7 +3759,7 @@
         <v>107</v>
       </c>
       <c r="N40" s="7" t="n">
-        <f aca="false">$B$96*C40</f>
+        <f aca="false">$B$95*C40</f>
         <v>255</v>
       </c>
       <c r="O40" s="7" t="n">
@@ -3785,14 +3810,14 @@
         <v>107</v>
       </c>
       <c r="N41" s="7" t="n">
-        <f aca="false">$B$96*C41</f>
+        <f aca="false">$B$95*C41</f>
         <v>680</v>
       </c>
       <c r="O41" s="7" t="n">
         <v>720</v>
       </c>
       <c r="P41" s="7" t="n">
-        <v>100</v>
+        <v>720</v>
       </c>
       <c r="R41" s="7" t="n">
         <v>0.067</v>
@@ -3833,7 +3858,7 @@
         <v>273</v>
       </c>
       <c r="N42" s="10" t="n">
-        <f aca="false">$B$96*C42</f>
+        <f aca="false">$B$95*C42</f>
         <v>170</v>
       </c>
       <c r="P42" s="10" t="n">
@@ -3895,7 +3920,7 @@
         <v>279</v>
       </c>
       <c r="N44" s="10" t="n">
-        <f aca="false">$B$96*C44</f>
+        <f aca="false">$B$95*C44</f>
         <v>170</v>
       </c>
       <c r="O44" s="10" t="n">
@@ -3937,7 +3962,7 @@
         <v>285</v>
       </c>
       <c r="N45" s="10" t="n">
-        <f aca="false">$B$96*C45</f>
+        <f aca="false">$B$95*C45</f>
         <v>170</v>
       </c>
       <c r="O45" s="10" t="n">
@@ -3979,7 +4004,7 @@
         <v>290</v>
       </c>
       <c r="N46" s="10" t="n">
-        <f aca="false">$B$96*C46</f>
+        <f aca="false">$B$95*C46</f>
         <v>765</v>
       </c>
       <c r="O46" s="10" t="n">
@@ -4024,7 +4049,7 @@
         <v>295</v>
       </c>
       <c r="N47" s="10" t="n">
-        <f aca="false">$B$96*C47</f>
+        <f aca="false">$B$95*C47</f>
         <v>85</v>
       </c>
       <c r="O47" s="10" t="n">
@@ -4086,7 +4111,7 @@
         <v>300</v>
       </c>
       <c r="N49" s="20" t="n">
-        <f aca="false">$B$96*C49</f>
+        <f aca="false">$B$95*C49</f>
         <v>255</v>
       </c>
       <c r="O49" s="20" t="n">
@@ -4127,7 +4152,7 @@
         <v>305</v>
       </c>
       <c r="N50" s="20" t="n">
-        <f aca="false">$B$96*C50</f>
+        <f aca="false">$B$95*C50</f>
         <v>255</v>
       </c>
       <c r="O50" s="20" t="n">
@@ -4153,7 +4178,7 @@
         <v>307</v>
       </c>
       <c r="N51" s="11" t="n">
-        <f aca="false">$B$96*C51</f>
+        <f aca="false">$B$95*C51</f>
         <v>0</v>
       </c>
       <c r="U51" s="11" t="s">
@@ -4163,25 +4188,43 @@
       <c r="AMI51" s="0"/>
       <c r="AMJ51" s="0"/>
     </row>
-    <row r="52" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="11" t="s">
+    <row r="52" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="C52" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" s="11" t="s">
+      <c r="C52" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G52" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="N52" s="11" t="n">
-        <f aca="false">$B$96*C52</f>
-        <v>0</v>
-      </c>
-      <c r="U52" s="11" t="s">
-        <v>69</v>
+      <c r="H52" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="L52" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="N52" s="10" t="n">
+        <f aca="false">$B$95*C52</f>
+        <v>85</v>
+      </c>
+      <c r="O52" s="10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="P52" s="10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U52" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="AI52" s="0"/>
       <c r="AMI52" s="0"/>
@@ -4189,32 +4232,32 @@
     </row>
     <row r="53" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>281</v>
       </c>
       <c r="C53" s="10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>276</v>
+        <v>313</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>270</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="N53" s="10" t="n">
-        <f aca="false">$B$96*C53</f>
-        <v>85</v>
+        <f aca="false">$B$95*C53</f>
+        <v>340</v>
       </c>
       <c r="O53" s="10" t="n">
         <v>5000</v>
@@ -4231,32 +4274,32 @@
     </row>
     <row r="54" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>281</v>
       </c>
       <c r="C54" s="10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>270</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="L54" s="10" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="N54" s="10" t="n">
-        <f aca="false">$B$96*C54</f>
-        <v>340</v>
+        <f aca="false">$B$95*C54</f>
+        <v>170</v>
       </c>
       <c r="O54" s="10" t="n">
         <v>5000</v>
@@ -4273,7 +4316,7 @@
     </row>
     <row r="55" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>281</v>
@@ -4282,22 +4325,22 @@
         <v>2</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>270</v>
+        <v>324</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="N55" s="10" t="n">
-        <f aca="false">$B$96*C55</f>
+        <f aca="false">$B$95*C55</f>
         <v>170</v>
       </c>
       <c r="O55" s="10" t="n">
@@ -4315,32 +4358,32 @@
     </row>
     <row r="56" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>281</v>
       </c>
       <c r="C56" s="10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>326</v>
+        <v>270</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="N56" s="10" t="n">
-        <f aca="false">$B$96*C56</f>
-        <v>170</v>
+        <f aca="false">$B$95*C56</f>
+        <v>595</v>
       </c>
       <c r="O56" s="10" t="n">
         <v>5000</v>
@@ -4355,194 +4398,209 @@
       <c r="AMI56" s="0"/>
       <c r="AMJ56" s="0"/>
     </row>
-    <row r="57" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>281</v>
       </c>
       <c r="C57" s="10" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>331</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="E57" s="10"/>
       <c r="F57" s="10" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="L57" s="10" t="s">
-        <v>334</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="M57" s="10"/>
       <c r="N57" s="10" t="n">
-        <f aca="false">$B$96*C57</f>
-        <v>595</v>
-      </c>
-      <c r="O57" s="10" t="n">
-        <v>5000</v>
-      </c>
-      <c r="P57" s="10" t="n">
-        <v>5000</v>
-      </c>
+        <f aca="false">$B$95*C57</f>
+        <v>1275</v>
+      </c>
+      <c r="O57" s="22" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P57" s="22" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Q57" s="10"/>
+      <c r="R57" s="10"/>
+      <c r="T57" s="10"/>
       <c r="U57" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI57" s="0"/>
-      <c r="AMI57" s="0"/>
+        <v>31</v>
+      </c>
+      <c r="V57" s="10"/>
+      <c r="AI57" s="10"/>
       <c r="AMJ57" s="0"/>
     </row>
-    <row r="58" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C58" s="10" t="n">
-        <v>15</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="G58" s="10" t="s">
+    <row r="58" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="H58" s="10" t="s">
+      <c r="B58" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10" t="n">
-        <f aca="false">$B$96*C58</f>
-        <v>1275</v>
-      </c>
-      <c r="O58" s="22" t="n">
-        <v>2000</v>
-      </c>
-      <c r="Q58" s="10"/>
-      <c r="R58" s="10"/>
-      <c r="T58" s="10"/>
-      <c r="U58" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="V58" s="10"/>
-      <c r="AI58" s="10"/>
+      <c r="C58" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="M58" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="N58" s="13" t="n">
+        <f aca="false">$B$95*C58</f>
+        <v>170</v>
+      </c>
+      <c r="O58" s="13" t="n">
+        <v>170</v>
+      </c>
+      <c r="P58" s="14" t="n">
+        <f aca="false">50+69+30+20</f>
+        <v>169</v>
+      </c>
+      <c r="Q58" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="T58" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="U58" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="AI58" s="0"/>
+      <c r="AMI58" s="0"/>
       <c r="AMJ58" s="0"/>
     </row>
     <row r="59" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="B59" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C59" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="F59" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="C59" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="F59" s="13" t="s">
-        <v>342</v>
-      </c>
       <c r="G59" s="13" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="I59" s="13" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>346</v>
+        <v>107</v>
       </c>
       <c r="N59" s="13" t="n">
-        <f aca="false">$B$96*C59</f>
-        <v>170</v>
+        <f aca="false">$B$95*C59</f>
+        <v>340</v>
       </c>
       <c r="O59" s="13" t="n">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="P59" s="14" t="n">
-        <f aca="false">50+69+30</f>
-        <v>149</v>
+        <f aca="false">340+32</f>
+        <v>372</v>
       </c>
       <c r="Q59" s="13" t="s">
         <v>114</v>
       </c>
+      <c r="R59" s="13" t="n">
+        <v>0.53</v>
+      </c>
       <c r="T59" s="13" t="s">
-        <v>347</v>
+        <v>108</v>
       </c>
       <c r="U59" s="13" t="s">
-        <v>348</v>
+        <v>172</v>
       </c>
       <c r="AI59" s="0"/>
       <c r="AMI59" s="0"/>
       <c r="AMJ59" s="0"/>
     </row>
-    <row r="60" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>350</v>
-      </c>
-      <c r="C60" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="F60" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="H60" s="13" t="s">
+    <row r="60" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="I60" s="13" t="s">
+      <c r="B60" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="M60" s="13" t="s">
+      <c r="C60" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="M60" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="N60" s="13" t="n">
-        <f aca="false">$B$96*C60</f>
-        <v>340</v>
-      </c>
-      <c r="O60" s="13" t="n">
-        <v>340</v>
-      </c>
-      <c r="P60" s="14" t="n">
-        <f aca="false">340+32</f>
-        <v>372</v>
-      </c>
-      <c r="Q60" s="13" t="s">
+      <c r="N60" s="7" t="n">
+        <f aca="false">$B$95*C60</f>
+        <v>170</v>
+      </c>
+      <c r="O60" s="7" t="n">
+        <v>170</v>
+      </c>
+      <c r="P60" s="7" t="n">
+        <v>170</v>
+      </c>
+      <c r="Q60" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="R60" s="13" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="T60" s="13" t="s">
+      <c r="R60" s="7" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="T60" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="U60" s="13" t="s">
-        <v>172</v>
+      <c r="U60" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="AI60" s="0"/>
       <c r="AMI60" s="0"/>
@@ -4550,50 +4608,50 @@
     </row>
     <row r="61" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C61" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="F61" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="C61" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>358</v>
-      </c>
       <c r="G61" s="7" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="M61" s="7" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="N61" s="7" t="n">
-        <f aca="false">$B$96*C61</f>
-        <v>170</v>
+        <f aca="false">$B$95*C61</f>
+        <v>85</v>
       </c>
       <c r="O61" s="7" t="n">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="P61" s="7" t="n">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="Q61" s="7" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="R61" s="7" t="n">
-        <v>0.18</v>
+        <v>2.84</v>
       </c>
       <c r="T61" s="7" t="s">
-        <v>108</v>
+        <v>366</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>31</v>
@@ -4602,309 +4660,312 @@
       <c r="AMI61" s="0"/>
       <c r="AMJ61" s="0"/>
     </row>
-    <row r="62" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="C62" s="7" t="n">
+    <row r="62" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="C62" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="I62" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="M62" s="7" t="s">
+      <c r="D62" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="M62" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="N62" s="7" t="n">
-        <f aca="false">$B$96*C62</f>
+      <c r="N62" s="10" t="n">
+        <f aca="false">$B$95*C62</f>
         <v>85</v>
       </c>
-      <c r="O62" s="7" t="n">
+      <c r="O62" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="P62" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q62" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="R62" s="7" t="n">
-        <v>2.84</v>
-      </c>
-      <c r="T62" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="U62" s="7" t="s">
-        <v>31</v>
+      <c r="P62" s="10" t="n">
+        <v>95</v>
+      </c>
+      <c r="T62" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="U62" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="AI62" s="0"/>
       <c r="AMI62" s="0"/>
       <c r="AMJ62" s="0"/>
     </row>
-    <row r="63" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="C63" s="10" t="n">
+    <row r="63" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="C63" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D63" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="H63" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="I63" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="L63" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="M63" s="10" t="s">
+      <c r="D63" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M63" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="N63" s="10" t="n">
-        <f aca="false">$B$96*C63</f>
+      <c r="N63" s="13" t="n">
+        <f aca="false">$B$95*C63</f>
         <v>85</v>
       </c>
-      <c r="O63" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="P63" s="10" t="n">
-        <v>95</v>
-      </c>
-      <c r="T63" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="U63" s="10" t="s">
-        <v>40</v>
+      <c r="O63" s="13" t="n">
+        <v>85</v>
+      </c>
+      <c r="P63" s="14" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q63" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="R63" s="13" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="T63" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="U63" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="AI63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
     </row>
-    <row r="64" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="C64" s="13" t="n">
+    <row r="64" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="C64" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="F64" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="G64" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="H64" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="I64" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="M64" s="13" t="s">
+      <c r="D64" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="L64" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="M64" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="N64" s="13" t="n">
-        <f aca="false">$B$96*C64</f>
+      <c r="N64" s="10" t="n">
+        <f aca="false">$B$95*C64</f>
         <v>85</v>
       </c>
-      <c r="O64" s="13" t="n">
-        <v>85</v>
-      </c>
-      <c r="P64" s="14" t="n">
-        <v>85</v>
-      </c>
-      <c r="Q64" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="R64" s="13" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="T64" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="U64" s="13" t="s">
-        <v>172</v>
+      <c r="O64" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="P64" s="10" t="n">
+        <v>95</v>
+      </c>
+      <c r="R64" s="10" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="T64" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="U64" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="AI64" s="0"/>
       <c r="AMI64" s="0"/>
       <c r="AMJ64" s="0"/>
     </row>
-    <row r="65" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="C65" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>388</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="E65" s="10"/>
       <c r="F65" s="10" t="s">
-        <v>389</v>
+        <v>356</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="I65" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="L65" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="M65" s="10" t="s">
-        <v>162</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="M65" s="10"/>
       <c r="N65" s="10" t="n">
-        <f aca="false">$B$96*C65</f>
         <v>85</v>
       </c>
-      <c r="O65" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="P65" s="10" t="n">
-        <v>95</v>
-      </c>
-      <c r="R65" s="10" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="T65" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="U65" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI65" s="0"/>
-      <c r="AMI65" s="0"/>
+      <c r="O65" s="22" t="n">
+        <v>85</v>
+      </c>
+      <c r="P65" s="22" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="10"/>
+      <c r="V65" s="10"/>
+      <c r="AI65" s="10"/>
       <c r="AMJ65" s="0"/>
     </row>
-    <row r="66" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="C66" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="G66" s="10" t="s">
+    <row r="66" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="H66" s="10" t="s">
+      <c r="B66" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="M66" s="10"/>
-      <c r="N66" s="10" t="n">
-        <v>85</v>
-      </c>
-      <c r="O66" s="22" t="n">
-        <v>85</v>
-      </c>
-      <c r="Q66" s="10"/>
-      <c r="R66" s="10"/>
-      <c r="T66" s="10"/>
-      <c r="U66" s="10"/>
-      <c r="V66" s="10"/>
-      <c r="AI66" s="10"/>
+      <c r="C66" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="M66" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="N66" s="7" t="n">
+        <f aca="false">$B$95*C66</f>
+        <v>425</v>
+      </c>
+      <c r="O66" s="7" t="n">
+        <v>500</v>
+      </c>
+      <c r="P66" s="7" t="n">
+        <v>500</v>
+      </c>
+      <c r="Q66" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="R66" s="7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="T66" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="U66" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI66" s="0"/>
+      <c r="AMI66" s="0"/>
       <c r="AMJ66" s="0"/>
     </row>
-    <row r="67" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="C67" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I67" s="7" t="s">
+    <row r="67" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="M67" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="N67" s="7" t="n">
-        <f aca="false">$B$96*C67</f>
-        <v>425</v>
-      </c>
-      <c r="O67" s="7" t="n">
-        <v>500</v>
-      </c>
-      <c r="P67" s="7" t="n">
-        <v>500</v>
-      </c>
-      <c r="Q67" s="7" t="s">
+      <c r="B67" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="C67" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="M67" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="N67" s="13" t="n">
+        <f aca="false">$B$95*C67</f>
+        <v>170</v>
+      </c>
+      <c r="O67" s="13" t="n">
+        <v>170</v>
+      </c>
+      <c r="P67" s="14" t="n">
+        <v>170</v>
+      </c>
+      <c r="Q67" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="R67" s="7" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="T67" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="U67" s="7" t="s">
-        <v>31</v>
+      <c r="R67" s="13" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="T67" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="U67" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="AI67" s="0"/>
       <c r="AMI67" s="0"/>
@@ -4912,34 +4973,34 @@
     </row>
     <row r="68" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C68" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>129</v>
+        <v>356</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="I68" s="13" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="M68" s="13" t="s">
         <v>172</v>
       </c>
       <c r="N68" s="13" t="n">
-        <f aca="false">$B$96*C68</f>
+        <f aca="false">$B$95*C68</f>
         <v>170</v>
       </c>
       <c r="O68" s="13" t="n">
@@ -4952,7 +5013,7 @@
         <v>114</v>
       </c>
       <c r="R68" s="13" t="n">
-        <v>0.15</v>
+        <v>1.4</v>
       </c>
       <c r="T68" s="13" t="s">
         <v>108</v>
@@ -4964,97 +5025,55 @@
       <c r="AMI68" s="0"/>
       <c r="AMJ68" s="0"/>
     </row>
-    <row r="69" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="13" t="s">
-        <v>411</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>412</v>
-      </c>
-      <c r="C69" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D69" s="13" t="s">
+    <row r="69" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="16" t="s">
         <v>413</v>
       </c>
-      <c r="F69" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="H69" s="13" t="s">
+      <c r="B69" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="I69" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="M69" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="N69" s="13" t="n">
-        <f aca="false">$B$96*C69</f>
-        <v>170</v>
-      </c>
-      <c r="O69" s="13" t="n">
-        <v>170</v>
-      </c>
-      <c r="P69" s="14" t="n">
-        <v>170</v>
-      </c>
-      <c r="Q69" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="R69" s="13" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="T69" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="U69" s="13" t="s">
-        <v>172</v>
+      <c r="C69" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="M69" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="N69" s="16" t="n">
+        <v>76</v>
+      </c>
+      <c r="O69" s="16" t="n">
+        <v>76</v>
+      </c>
+      <c r="P69" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="T69" s="16" t="s">
+        <v>420</v>
       </c>
       <c r="AI69" s="0"/>
       <c r="AMI69" s="0"/>
       <c r="AMJ69" s="0"/>
     </row>
-    <row r="70" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="16" t="s">
-        <v>415</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="C70" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D70" s="16" t="s">
-        <v>417</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>418</v>
-      </c>
-      <c r="G70" s="16" t="s">
-        <v>419</v>
-      </c>
-      <c r="M70" s="16" t="s">
-        <v>420</v>
-      </c>
-      <c r="N70" s="16" t="n">
-        <v>76</v>
-      </c>
-      <c r="O70" s="16" t="n">
-        <v>76</v>
-      </c>
-      <c r="P70" s="17" t="n">
-        <v>71</v>
-      </c>
-      <c r="T70" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="AI70" s="0"/>
-      <c r="AMI70" s="0"/>
-      <c r="AMJ70" s="0"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G70" s="0"/>
+      <c r="H70" s="0"/>
+      <c r="I70" s="0"/>
+      <c r="J70" s="0"/>
+      <c r="K70" s="0"/>
+      <c r="N70" s="0" t="n">
+        <f aca="false">$B$95*C70</f>
+        <v>0</v>
+      </c>
+      <c r="R70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G71" s="0"/>
@@ -5063,118 +5082,143 @@
       <c r="J71" s="0"/>
       <c r="K71" s="0"/>
       <c r="N71" s="0" t="n">
-        <f aca="false">$B$96*C71</f>
+        <f aca="false">$B$95*C71</f>
         <v>0</v>
       </c>
       <c r="R71" s="0"/>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G72" s="0"/>
-      <c r="H72" s="0"/>
-      <c r="I72" s="0"/>
-      <c r="J72" s="0"/>
-      <c r="K72" s="0"/>
-      <c r="N72" s="0" t="n">
-        <f aca="false">$B$96*C72</f>
+    <row r="72" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="23" t="s">
+        <v>421</v>
+      </c>
+      <c r="C72" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="D72" s="24" t="n">
+        <v>1282.1501</v>
+      </c>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="G72" s="24" t="n">
+        <v>1282.1501</v>
+      </c>
+      <c r="J72" s="23" t="n">
+        <v>2300599</v>
+      </c>
+      <c r="N72" s="23" t="n">
+        <f aca="false">$B$95*C72</f>
+        <v>255</v>
+      </c>
+      <c r="O72" s="23" t="n">
+        <v>300</v>
+      </c>
+      <c r="P72" s="25" t="n">
+        <v>277</v>
+      </c>
+      <c r="R72" s="23" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="T72" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="U72" s="23" t="s">
+        <v>423</v>
+      </c>
+      <c r="AMI72" s="0"/>
+      <c r="AMJ72" s="0"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="N73" s="0" t="n">
+        <f aca="false">$B$95*C73</f>
         <v>0</v>
       </c>
-      <c r="R72" s="0"/>
-    </row>
-    <row r="73" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="23" t="s">
-        <v>422</v>
-      </c>
-      <c r="C73" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D73" s="24" t="n">
-        <v>1282.1501</v>
-      </c>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24" t="s">
-        <v>423</v>
-      </c>
-      <c r="G73" s="24" t="n">
-        <v>1282.1501</v>
-      </c>
-      <c r="J73" s="23" t="n">
-        <v>2300599</v>
-      </c>
-      <c r="N73" s="23" t="n">
-        <f aca="false">$B$96*C73</f>
-        <v>255</v>
-      </c>
-      <c r="O73" s="23" t="n">
-        <v>300</v>
-      </c>
-      <c r="P73" s="25"/>
-      <c r="R73" s="23" t="n">
-        <v>1.16</v>
-      </c>
-      <c r="T73" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="U73" s="23" t="s">
-        <v>424</v>
-      </c>
-      <c r="AMI73" s="0"/>
-      <c r="AMJ73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="F74" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="F74" s="0" t="s">
-        <v>426</v>
-      </c>
       <c r="G74" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="N74" s="0" t="n">
-        <f aca="false">$B$96*C74</f>
+        <f aca="false">$B$95*C74</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>428</v>
-      </c>
-      <c r="F75" s="0" t="s">
-        <v>426</v>
-      </c>
-      <c r="N75" s="0" t="n">
-        <f aca="false">$B$96*C75</f>
-        <v>0</v>
-      </c>
+    <row r="75" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="C75" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="H75" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="N75" s="7" t="n">
+        <f aca="false">$B$95*C75</f>
+        <v>425</v>
+      </c>
+      <c r="O75" s="7" t="n">
+        <v>500</v>
+      </c>
+      <c r="P75" s="9" t="n">
+        <v>500</v>
+      </c>
+      <c r="R75" s="8"/>
+      <c r="U75" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AMI75" s="9"/>
+      <c r="AMJ75" s="9"/>
     </row>
     <row r="76" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="C76" s="7" t="n">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>153</v>
       </c>
       <c r="G76" s="19" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="H76" s="19" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="I76" s="19"/>
       <c r="J76" s="19"/>
       <c r="K76" s="19"/>
       <c r="N76" s="7" t="n">
-        <f aca="false">$B$96*C76</f>
-        <v>425</v>
+        <v>85</v>
       </c>
       <c r="O76" s="7" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="P76" s="9" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="R76" s="8"/>
       <c r="U76" s="7" t="s">
@@ -5185,30 +5229,35 @@
     </row>
     <row r="77" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G77" s="19" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="H77" s="19" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="I77" s="19"/>
       <c r="J77" s="19"/>
       <c r="K77" s="19"/>
       <c r="N77" s="7" t="n">
+        <v>75</v>
+      </c>
+      <c r="O77" s="7" t="n">
         <v>85</v>
       </c>
-      <c r="O77" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="P77" s="9" t="n">
-        <v>100</v>
-      </c>
-      <c r="R77" s="8"/>
+      <c r="P77" s="7" t="n">
+        <v>78</v>
+      </c>
+      <c r="R77" s="8" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="T77" s="7" t="s">
+        <v>438</v>
+      </c>
       <c r="U77" s="7" t="s">
         <v>31</v>
       </c>
@@ -5217,136 +5266,135 @@
     </row>
     <row r="78" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>159</v>
       </c>
       <c r="G78" s="19" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="H78" s="19" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="I78" s="19"/>
       <c r="J78" s="19"/>
       <c r="K78" s="19"/>
-      <c r="N78" s="7" t="n">
-        <v>75</v>
-      </c>
-      <c r="O78" s="7" t="n">
-        <v>85</v>
-      </c>
-      <c r="R78" s="8" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="T78" s="7" t="s">
-        <v>438</v>
-      </c>
+      <c r="R78" s="8"/>
       <c r="U78" s="7" t="s">
         <v>31</v>
       </c>
       <c r="AMI78" s="9"/>
       <c r="AMJ78" s="9"/>
     </row>
-    <row r="79" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G79" s="19" t="s">
-        <v>440</v>
-      </c>
-      <c r="H79" s="19" t="s">
-        <v>441</v>
-      </c>
-      <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
-      <c r="K79" s="19"/>
-      <c r="R79" s="8"/>
-      <c r="U79" s="7" t="s">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="G79" s="0"/>
+      <c r="H79" s="0"/>
+      <c r="I79" s="0"/>
+      <c r="J79" s="0"/>
+      <c r="K79" s="0"/>
+      <c r="R79" s="0"/>
+    </row>
+    <row r="80" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="G80" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="H80" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+      <c r="M80" s="7"/>
+      <c r="N80" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="O80" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="P80" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q80" s="7"/>
+      <c r="R80" s="8" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="T80" s="7"/>
+      <c r="U80" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AMI79" s="9"/>
-      <c r="AMJ79" s="9"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>442</v>
-      </c>
-      <c r="G80" s="0"/>
-      <c r="H80" s="0"/>
-      <c r="I80" s="0"/>
-      <c r="J80" s="0"/>
-      <c r="K80" s="0"/>
-      <c r="R80" s="0"/>
-    </row>
-    <row r="81" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7" t="n">
+      <c r="V80" s="7"/>
+      <c r="AI80" s="7"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C81" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="G81" s="19" t="s">
-        <v>445</v>
-      </c>
-      <c r="H81" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="I81" s="19"/>
-      <c r="J81" s="19"/>
-      <c r="K81" s="19"/>
-      <c r="M81" s="7"/>
-      <c r="N81" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="O81" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q81" s="7"/>
-      <c r="R81" s="8" t="n">
-        <v>1.31</v>
-      </c>
-      <c r="T81" s="7"/>
-      <c r="U81" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="V81" s="7"/>
-      <c r="AI81" s="7"/>
+      <c r="F81" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="N81" s="0" t="n">
+        <f aca="false">$B$95*C81</f>
+        <v>85</v>
+      </c>
+      <c r="P81" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="U81" s="0" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="N82" s="0" t="n">
-        <f aca="false">$B$96*C82</f>
-        <v>85</v>
+        <f aca="false">$B$95*C82</f>
+        <v>510</v>
+      </c>
+      <c r="O82" s="0" t="n">
+        <v>1000</v>
       </c>
       <c r="P82" s="0" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="U82" s="0" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>6</v>
@@ -5355,13 +5403,10 @@
         <v>450</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="N83" s="0" t="n">
-        <f aca="false">$B$96*C83</f>
+        <f aca="false">$B$95*C83</f>
         <v>510</v>
       </c>
       <c r="O83" s="0" t="n">
@@ -5376,158 +5421,166 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="C84" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F84" s="0" t="s">
-        <v>450</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="N84" s="0" t="n">
-        <f aca="false">$B$96*C84</f>
-        <v>510</v>
-      </c>
-      <c r="O84" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="P84" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U84" s="0" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="86" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="9" t="s">
+    <row r="85" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="F86" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="G86" s="9" t="n">
+      <c r="C85" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="G85" s="9" t="n">
         <v>687720100002</v>
       </c>
-      <c r="N86" s="7" t="n">
-        <f aca="false">$B$96*C86</f>
-        <v>0</v>
-      </c>
-      <c r="U86" s="9" t="s">
+      <c r="N85" s="7" t="n">
+        <f aca="false">$B$95*C85</f>
+        <v>85</v>
+      </c>
+      <c r="U85" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="V86" s="9" t="s">
+      <c r="V85" s="9" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
         <v>459</v>
       </c>
-      <c r="N87" s="0" t="n">
-        <f aca="false">$B$96*C87</f>
-        <v>0</v>
+      <c r="C86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N86" s="0" t="n">
+        <f aca="false">$B$95*C86</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="C87" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="G87" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="H87" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="I87" s="19"/>
+      <c r="J87" s="19"/>
+      <c r="K87" s="19"/>
+      <c r="N87" s="9" t="n">
+        <v>80</v>
+      </c>
+      <c r="O87" s="9" t="n">
+        <v>80</v>
+      </c>
+      <c r="R87" s="8"/>
+      <c r="U87" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N88" s="0" t="n">
-        <f aca="false">$B$96*C88</f>
+        <f aca="false">$B$95*C88</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N89" s="0" t="n">
-        <f aca="false">$B$96*C89</f>
+        <f aca="false">$B$95*C89</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N90" s="0" t="n">
-        <f aca="false">$B$96*C90</f>
+        <f aca="false">$B$95*C90</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N91" s="0" t="n">
-        <f aca="false">$B$96*C91</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="C92" s="0" t="n">
+      <c r="B91" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="C91" s="0" t="n">
         <v>1.38</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="B96" s="0" t="n">
         <v>85</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="B98" s="0" t="s">
-        <v>465</v>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="10" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="10" t="s">
-        <v>466</v>
+      <c r="A100" s="7" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="s">
-        <v>467</v>
+      <c r="A101" s="13" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="13" t="s">
-        <v>468</v>
+      <c r="A102" s="23" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="23" t="s">
-        <v>469</v>
+      <c r="A103" s="20" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="20" t="s">
-        <v>470</v>
+      <c r="A104" s="26" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5536,7 +5589,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P87:P91 P81:P85 P2:P79">
+  <conditionalFormatting sqref="P86:P90 P80:P84 P2:P78">
     <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>'safeproject-panel-r2-bom-21340'!N2</formula>
     </cfRule>

</xml_diff>